<commit_message>
Carga Masiva de Animales
</commit_message>
<xml_diff>
--- a/extensiones/excel/cargas/Ovejas Gianni1.xlsx
+++ b/extensiones/excel/cargas/Ovejas Gianni1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7F4A14-51CB-4C92-AE79-69DC04AAA9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C3E9A0-88F3-4A83-888B-E2E3FB288956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2545250A-E0BE-443A-B961-C47292E8FB53}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="48">
   <si>
     <t>Numero Caravana</t>
   </si>
@@ -147,14 +147,38 @@
     <t>Servida</t>
   </si>
   <si>
-    <t>Complicacion</t>
+    <t>PAMPERITO</t>
+  </si>
+  <si>
+    <t>NARANJA ( villa maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NARANJA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NARANJA </t>
+  </si>
+  <si>
+    <t>AMARILLA NUEVA</t>
+  </si>
+  <si>
+    <t>AMARILLA  QUEDO</t>
+  </si>
+  <si>
+    <t>QUEDO AMARILLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BORREGA </t>
+  </si>
+  <si>
+    <t>BORREGA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +193,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,8 +220,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -223,19 +260,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -284,22 +308,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,23 +333,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,26 +342,56 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,19 +706,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1B918A-3D56-4D49-9575-605714E69FBF}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="21"/>
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -705,234 +734,227 @@
       <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>87</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="18"/>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>71</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>6</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>61</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
         <v>23</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>64</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>66</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>39</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>62</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>83</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>88</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>70</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>71</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>12</v>
-      </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>13</v>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -946,11 +968,10 @@
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>45</v>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
@@ -959,16 +980,15 @@
         <v>3</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>54</v>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
+        <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
@@ -977,106 +997,98 @@
         <v>3</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
+        <v>28</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
+        <v>32</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="23">
+        <v>34</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="23">
+        <v>35</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>9</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>25</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>91</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>74</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>80</v>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
+        <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>4</v>
@@ -1090,14 +1102,13 @@
       <c r="E23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>76</v>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23">
+        <v>37</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>3</v>
@@ -1108,10 +1119,9 @@
       <c r="E24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="23">
         <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1126,11 +1136,10 @@
       <c r="E25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>11</v>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>4</v>
@@ -1138,17 +1147,14 @@
       <c r="C26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D26" s="4"/>
       <c r="E26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>37</v>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>4</v>
@@ -1157,15 +1163,14 @@
         <v>3</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="23">
         <v>43</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -1180,11 +1185,10 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>8</v>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
+        <v>44</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>4</v>
@@ -1193,34 +1197,32 @@
         <v>3</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="23">
+        <v>45</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="23">
         <v>48</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>44</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>4</v>
@@ -1234,11 +1236,10 @@
       <c r="E31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>67</v>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
+        <v>49</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>4</v>
@@ -1247,35 +1248,35 @@
         <v>3</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>30</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="23">
+        <v>51</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>78</v>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="23">
+        <v>54</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>3</v>
@@ -1286,11 +1287,10 @@
       <c r="E34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>92</v>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>55</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>4</v>
@@ -1304,11 +1304,10 @@
       <c r="E35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>51</v>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="23">
+        <v>57</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>4</v>
@@ -1317,124 +1316,109 @@
         <v>3</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="23">
+        <v>58</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>18</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="E37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>77</v>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="23">
+        <v>59</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>55</v>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="23">
+        <v>61</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D39" s="4"/>
       <c r="E39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>28</v>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="23">
+        <v>62</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D40" s="4"/>
       <c r="E40" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>49</v>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="23">
+        <v>64</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="D41" s="4"/>
       <c r="E41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>36</v>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="23">
+        <v>66</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D42" s="4"/>
       <c r="E42" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>24</v>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="23">
+        <v>67</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>4</v>
@@ -1443,19 +1427,18 @@
         <v>3</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>17</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>4</v>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="23">
+        <v>70</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>3</v>
@@ -1466,11 +1449,10 @@
       <c r="E44" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>90</v>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="23">
+        <v>71</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>4</v>
@@ -1478,51 +1460,48 @@
       <c r="C45" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="4"/>
+      <c r="E45" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="23">
+        <v>71</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>80</v>
-      </c>
-      <c r="B46" s="4" t="s">
+      <c r="E46" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="22">
+        <v>72</v>
+      </c>
+      <c r="B47" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>81</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>16</v>
+      <c r="C47" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>27</v>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="23">
+        <v>74</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>4</v>
@@ -1536,14 +1515,13 @@
       <c r="E48" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
-        <v>82</v>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="23">
+        <v>76</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>3</v>
@@ -1554,50 +1532,47 @@
       <c r="E49" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>99</v>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="23">
+        <v>77</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>41</v>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="23">
+        <v>78</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>84</v>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="23">
+        <v>80</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>3</v>
@@ -1608,189 +1583,937 @@
       <c r="E52" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>59</v>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="23">
+        <v>80</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="D53" s="4"/>
       <c r="E53" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>22</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="4" t="s">
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="24">
+        <v>81</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="23">
+        <v>82</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="23">
+        <v>83</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="23">
+        <v>84</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="23">
+        <v>85</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="23">
+        <v>86</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
-        <v>34</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="E59" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="23">
+        <v>87</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="23">
+        <v>88</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="E61" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="23">
+        <v>90</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="23">
+        <v>91</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="23">
+        <v>92</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="23">
+        <v>99</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="22"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="22">
+        <v>92</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="22">
+        <v>61</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="22">
+        <v>62</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="22">
+        <v>98</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="5"/>
+      <c r="E70" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="22">
+        <v>96</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="22">
+        <v>2</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="22">
+        <v>90</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="22">
+        <v>37</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="22">
+        <v>89</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="5"/>
+      <c r="E75" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="19">
+        <v>63</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="19">
+        <v>64</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="19">
+        <v>65</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="19">
+        <v>66</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="19">
+        <v>67</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="19">
+        <v>68</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="19">
+        <v>72</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="19">
+        <v>73</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="19">
+        <v>75</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="19">
+        <v>76</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="19">
+        <v>77</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="19">
+        <v>78</v>
+      </c>
+      <c r="B87" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="19">
+        <v>79</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="19">
+        <v>81</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="19">
+        <v>82</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="19">
+        <v>84</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="19">
         <v>85</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B92" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="19">
+        <v>86</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="19">
+        <v>89</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="19">
+        <v>94</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="19">
+        <v>95</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="19">
+        <v>21</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="19">
+        <v>19</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="19">
+        <v>12</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="19">
+        <v>16</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="19">
+        <v>18</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="19">
+        <v>24</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="19">
+        <v>17</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="19">
+        <v>10</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="19">
+        <v>41</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="19">
+        <v>36</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D106" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="19">
+        <v>31</v>
+      </c>
+      <c r="B107" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="19">
         <v>9</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
-        <v>58</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
-        <v>14</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
-        <v>35</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
-        <v>86</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
-        <v>57</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
-        <v>32</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F62" s="2"/>
+      <c r="B108" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E70">
+    <sortCondition ref="A4:A70"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1798,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427E3240-BB95-4582-9C3C-71FF70D226A4}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,63 +2535,58 @@
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1877,16 +2595,15 @@
       <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1895,16 +2612,15 @@
       <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1913,16 +2629,15 @@
       <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1931,16 +2646,15 @@
       <c r="D7" s="4">
         <v>6</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1949,16 +2663,15 @@
       <c r="D8" s="4">
         <v>6</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1967,16 +2680,15 @@
       <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1985,16 +2697,15 @@
       <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -2003,16 +2714,15 @@
       <c r="D11" s="4">
         <v>6</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2021,16 +2731,15 @@
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2039,16 +2748,15 @@
       <c r="D13" s="4">
         <v>2</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -2057,16 +2765,15 @@
       <c r="D14" s="4">
         <v>4</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -2075,16 +2782,15 @@
       <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2093,16 +2799,15 @@
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2111,16 +2816,15 @@
       <c r="D17" s="4">
         <v>2</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2129,16 +2833,15 @@
       <c r="D18" s="4">
         <v>4</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -2147,16 +2850,15 @@
       <c r="D19" s="4">
         <v>4</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2165,16 +2867,15 @@
       <c r="D20" s="4">
         <v>3</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -2183,16 +2884,15 @@
       <c r="D21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -2201,16 +2901,15 @@
       <c r="D22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -2219,16 +2918,15 @@
       <c r="D23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -2237,16 +2935,15 @@
       <c r="D24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -2255,16 +2952,15 @@
       <c r="D25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -2273,16 +2969,15 @@
       <c r="D26" s="4">
         <v>6</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -2291,16 +2986,15 @@
       <c r="D27" s="4">
         <v>6</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="28" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -2309,10 +3003,9 @@
       <c r="D28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2324,7 +3017,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,39 +3029,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2381,7 +3074,7 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2398,7 +3091,7 @@
       <c r="D4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2415,7 +3108,7 @@
       <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2428,7 +3121,7 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2445,7 +3138,7 @@
       <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2462,7 +3155,7 @@
       <c r="D8" s="6">
         <v>6</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2479,7 +3172,7 @@
       <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2496,7 +3189,7 @@
       <c r="D10" s="6">
         <v>4</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2513,7 +3206,7 @@
       <c r="D11" s="6">
         <v>6</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2530,7 +3223,7 @@
       <c r="D12" s="6">
         <v>6</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2547,7 +3240,7 @@
       <c r="D13" s="6">
         <v>6</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2564,7 +3257,7 @@
       <c r="D14" s="6">
         <v>6</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2581,7 +3274,7 @@
       <c r="D15" s="6">
         <v>6</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2598,7 +3291,7 @@
       <c r="D16" s="6">
         <v>6</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2615,7 +3308,7 @@
       <c r="D17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2632,7 +3325,7 @@
       <c r="D18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2649,7 +3342,7 @@
       <c r="D19" s="6">
         <v>6</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2666,7 +3359,7 @@
       <c r="D20" s="6">
         <v>6</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2683,7 +3376,7 @@
       <c r="D21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2700,7 +3393,7 @@
       <c r="D22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2717,7 +3410,7 @@
       <c r="D23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2734,7 +3427,7 @@
       <c r="D24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2751,7 +3444,7 @@
       <c r="D25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2766,7 +3459,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2781,7 +3474,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2798,7 +3491,7 @@
       <c r="D28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2815,7 +3508,7 @@
       <c r="D29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2832,7 +3525,7 @@
       <c r="D30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2849,7 +3542,7 @@
       <c r="D31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2860,10 +3553,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978FC54D-0ECF-42DC-B7F1-6436752B65FF}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2872,44 +3565,41 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="16">
+      <c r="C2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11">
         <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2926,7 +3616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2943,7 +3633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2960,7 +3650,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2977,7 +3667,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2994,7 +3684,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -3011,7 +3701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3028,7 +3718,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>35</v>
       </c>

</xml_diff>